<commit_message>
updating docs - preview2
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-Procedure-blood-transfusion.xlsx
+++ b/docs/StructureDefinition-Procedure-blood-transfusion.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-05T09:43:17-05:00</t>
+    <t>2024-05-01T14:05:02-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -3605,7 +3605,7 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" t="s" s="2">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>87</v>

</xml_diff>